<commit_message>
Updated with Robbies files
</commit_message>
<xml_diff>
--- a/tilburg tables.xlsx
+++ b/tilburg tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chjh\Dropbox\projects\2014rpp\master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Werk\Onderzoek\Reproducibility project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="111">
   <si>
     <t>Correlations and CIs</t>
   </si>
@@ -354,6 +354,42 @@
   <si>
     <t>1 / 6</t>
   </si>
+  <si>
+    <t>0.356 (0.292)</t>
+  </si>
+  <si>
+    <t>0.138 (0.076)</t>
+  </si>
+  <si>
+    <t>0.45 (0.273)</t>
+  </si>
+  <si>
+    <t>0.339 (0.292)</t>
+  </si>
+  <si>
+    <t>0.587 (0.389)</t>
+  </si>
+  <si>
+    <t>0.489 (0.300)</t>
+  </si>
+  <si>
+    <t>42,0</t>
+  </si>
+  <si>
+    <t>15,8</t>
+  </si>
+  <si>
+    <t>61,9</t>
+  </si>
+  <si>
+    <t>31,3</t>
+  </si>
+  <si>
+    <t>57,1</t>
+  </si>
+  <si>
+    <t>66,7</t>
+  </si>
 </sst>
 </file>
 
@@ -462,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -510,9 +546,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -529,17 +562,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,6 +575,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -634,6 +676,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="10048875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -936,7 +1026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -947,16 +1037,16 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="28" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="28" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="29"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="9"/>
@@ -1027,33 +1117,37 @@
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="27" t="s">
         <v>85</v>
       </c>
       <c r="C3" s="17">
         <v>0.33</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="19">
-        <v>0.78900000000000003</v>
+      <c r="F3" s="37" t="s">
+        <v>99</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="G3" s="39">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>105</v>
+      </c>
       <c r="I3" s="17">
         <f>36/(36+56)</f>
         <v>0.39130434782608697</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="34"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -1063,106 +1157,136 @@
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="30">
         <v>0.17</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="F5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="13">
+        <v>47.4</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>106</v>
+      </c>
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="30">
         <v>0.46</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="F6" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="13">
+        <v>85.7</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>107</v>
+      </c>
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="30">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="F7" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="13">
+        <v>68.8</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>108</v>
+      </c>
       <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="30">
         <v>0.67</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="F8" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="13">
+        <v>100</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>109</v>
+      </c>
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="31">
         <v>0.17</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
+      <c r="F9" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="22">
+        <v>83.3</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -1317,7 +1441,7 @@
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -1515,7 +1639,7 @@
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="25"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
@@ -1526,7 +1650,7 @@
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="26"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -11213,26 +11337,26 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="30" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="30" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="31"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
@@ -11577,11 +11701,11 @@
       <c r="D21" s="10"/>
       <c r="E21" s="12"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="20"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13"/>
@@ -11591,26 +11715,26 @@
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32" t="s">
+      <c r="E23" s="35"/>
+      <c r="F23" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="32" t="s">
+      <c r="G23" s="35"/>
+      <c r="H23" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="32" t="s">
+      <c r="I23" s="35"/>
+      <c r="J23" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="K23" s="31"/>
+      <c r="K23" s="35"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13"/>
@@ -18526,26 +18650,26 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="30" t="s">
+      <c r="J1" s="35"/>
+      <c r="K1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="30" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="31"/>
+      <c r="N1" s="35"/>
       <c r="O1" s="3" t="s">
         <v>6</v>
       </c>
@@ -18922,11 +19046,11 @@
       <c r="G19" s="10"/>
       <c r="H19" s="12"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="20"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="19"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13"/>
@@ -18942,26 +19066,26 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32" t="s">
+      <c r="F21" s="35"/>
+      <c r="G21" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32" t="s">
+      <c r="H21" s="35"/>
+      <c r="I21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="32" t="s">
+      <c r="J21" s="35"/>
+      <c r="K21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="32" t="s">
+      <c r="L21" s="35"/>
+      <c r="M21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="N21" s="31"/>
+      <c r="N21" s="35"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13"/>
@@ -28819,26 +28943,26 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="30" t="s">
+      <c r="J1" s="35"/>
+      <c r="K1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="30" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="31"/>
+      <c r="N1" s="35"/>
       <c r="O1" s="3" t="s">
         <v>6</v>
       </c>
@@ -29240,26 +29364,26 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32" t="s">
+      <c r="F21" s="35"/>
+      <c r="G21" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32" t="s">
+      <c r="H21" s="35"/>
+      <c r="I21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="32" t="s">
+      <c r="J21" s="35"/>
+      <c r="K21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="L21" s="31"/>
-      <c r="M21" s="32" t="s">
+      <c r="L21" s="35"/>
+      <c r="M21" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="N21" s="31"/>
+      <c r="N21" s="35"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13"/>

</xml_diff>

<commit_message>
Corrected value in tables
</commit_message>
<xml_diff>
--- a/tilburg tables.xlsx
+++ b/tilburg tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Werk\Onderzoek\Reproducibility project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chjh\Dropbox\projects\2014rpp\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -344,9 +344,6 @@
     <t>0.39 (0.19)</t>
   </si>
   <si>
-    <t>0.39 (0.24)</t>
-  </si>
-  <si>
     <t>0.37 (0.21)</t>
   </si>
   <si>
@@ -414,6 +411,9 @@
   </si>
   <si>
     <t>0.429 (0.236)</t>
+  </si>
+  <si>
+    <t>0.21 (0.24)</t>
   </si>
 </sst>
 </file>
@@ -842,6 +842,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="10048875"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1112,7 +1160,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1212,17 +1260,17 @@
       <c r="D3" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>87</v>
+      <c r="E3" s="32" t="s">
+        <v>110</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" s="34">
         <v>0.72499999999999998</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I3" s="17">
         <f>36/(36+56)</f>
@@ -1244,7 +1292,7 @@
         <v>70</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="30">
         <v>0.17</v>
@@ -1256,13 +1304,13 @@
         <v>82</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="13">
         <v>47.4</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="13"/>
     </row>
@@ -1271,7 +1319,7 @@
         <v>71</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="30">
         <v>0.46</v>
@@ -1283,13 +1331,13 @@
         <v>84</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G6" s="13">
         <v>85.7</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I6" s="13"/>
     </row>
@@ -1298,25 +1346,25 @@
         <v>72</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="30">
         <v>0.28999999999999998</v>
       </c>
       <c r="D7" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>89</v>
-      </c>
       <c r="F7" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="13">
         <v>68.8</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I7" s="13"/>
     </row>
@@ -1325,25 +1373,25 @@
         <v>73</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="30">
         <v>0.67</v>
       </c>
       <c r="D8" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>91</v>
-      </c>
       <c r="F8" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="13">
         <v>100</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" s="13"/>
     </row>
@@ -1352,25 +1400,25 @@
         <v>74</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="31">
         <v>0.17</v>
       </c>
       <c r="D9" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>93</v>
-      </c>
       <c r="F9" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" s="22">
         <v>83.3</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I9" s="22"/>
     </row>

</xml_diff>

<commit_message>
Adjusted small error in F3 table cell sheet 1
</commit_message>
<xml_diff>
--- a/tilburg tables.xlsx
+++ b/tilburg tables.xlsx
@@ -434,9 +434,6 @@
     <t>0.29 (0.19)</t>
   </si>
   <si>
-    <t>0.29 (0.25)</t>
-  </si>
-  <si>
     <t>0.14 (0.44)</t>
   </si>
   <si>
@@ -480,6 +477,9 @@
   </si>
   <si>
     <t>0.408 (0.263)</t>
+  </si>
+  <si>
+    <t>0.2 (0.25)</t>
   </si>
 </sst>
 </file>
@@ -1491,9 +1491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1611,7 +1611,7 @@
         <v>56</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="G3" s="32">
         <v>70</v>
@@ -1620,7 +1620,7 @@
         <v>0.91800000000000004</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J3" s="34">
         <v>0.70599999999999996</v>
@@ -1672,13 +1672,13 @@
         <v>0.89900000000000002</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5" s="40">
         <v>42.1</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L5" s="40"/>
     </row>
@@ -1687,19 +1687,19 @@
         <v>71</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="30">
         <v>0.46</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="40">
         <v>38</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="40">
         <v>41</v>
@@ -1708,7 +1708,7 @@
         <v>0.93300000000000005</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J6" s="40">
         <v>86.4</v>
@@ -1735,7 +1735,7 @@
         <v>83</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" s="40">
         <v>135</v>
@@ -1744,7 +1744,7 @@
         <v>0.91200000000000003</v>
       </c>
       <c r="I7" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J7" s="40">
         <v>64.3</v>
@@ -1759,19 +1759,19 @@
         <v>73</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" s="30">
         <v>0.7</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" s="40">
         <v>22</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G8" s="40">
         <v>25</v>
@@ -1780,7 +1780,7 @@
         <v>0.97399999999999998</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J8" s="40">
         <v>100</v>
@@ -1807,7 +1807,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="22">
         <v>13</v>
@@ -1816,7 +1816,7 @@
         <v>0.85</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J9" s="22">
         <v>80</v>

</xml_diff>